<commit_message>
App Auth Method added
</commit_message>
<xml_diff>
--- a/Data/TransactionData.xlsx
+++ b/Data/TransactionData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LuisRamos\OneDrive - Roboyo Global\Documents\UiPath\Personal\BotMonitor\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA133C6-CD3B-4C4F-ACC4-31AD3863A1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F9E987-A489-42AF-A929-A11950A97D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -76,16 +76,16 @@
     <x:t>CNB</x:t>
   </x:si>
   <x:si>
-    <x:t>https://cloud.uipath.com/cnbfl/cnbfl/orchestrator_/</x:t>
+    <x:t>https://cloud.uipath.com/cnbfl/cnbfl_dev/orchestrator_/</x:t>
   </x:si>
   <x:si>
-    <x:t>cnbfl</x:t>
+    <x:t>cnbfl_dev</x:t>
   </x:si>
   <x:si>
     <x:t>Failed</x:t>
   </x:si>
   <x:si>
-    <x:t>Business exception: Something happend during authentication... at Source: Orchestrator_CloudAuthentication - Invoke Workflow File (Process\Orchestrator\Orchestrator_CloudAuthentication.xaml): Throw - Not Cloud</x:t>
+    <x:t>Business exception: Something happend during authentication... at Source: Orchestrator_GetFolders - Invoke Workflow File (Process\Orchestrator\Orchestrator_GetFolders.xaml): Throw - Not Cloud</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -497,16 +497,16 @@
   <x:dimension ref="A1:BQ234"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="D19" sqref="D19"/>
+      <x:selection activeCell="F4" sqref="F4"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="67.525781" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <x:sheetFormatPr defaultColWidth="95.991406" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:cols>
     <x:col min="1" max="1" width="10.554688" style="0" bestFit="1" customWidth="1"/>
     <x:col min="2" max="2" width="54.777344" style="0" bestFit="1" customWidth="1"/>
     <x:col min="3" max="3" width="15.441406" style="0" bestFit="1" customWidth="1"/>
     <x:col min="4" max="4" width="11.554688" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="5" max="6" width="29.152031" style="0" customWidth="1"/>
+    <x:col min="5" max="6" width="29.109375" style="0" customWidth="1"/>
     <x:col min="7" max="7" width="0" style="0" hidden="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>

</xml_diff>